<commit_message>
Almost all parameters added
</commit_message>
<xml_diff>
--- a/data/Inputs.xlsx
+++ b/data/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3dd903d477a9e4d/02_ME/ME54015/OWF_Vessel-Fleet-Optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="174" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8075812-09FF-44AA-9110-6158957EF36A}"/>
+  <xr:revisionPtr revIDLastSave="207" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6287613-7D4E-4B18-B165-7B7CE9C12CF1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>B1</t>
   </si>
@@ -156,6 +156,24 @@
   </si>
   <si>
     <t>cost_purchase</t>
+  </si>
+  <si>
+    <t>cost_operation</t>
+  </si>
+  <si>
+    <t>cost_technicians</t>
+  </si>
+  <si>
+    <t>cost_downtime</t>
+  </si>
+  <si>
+    <t>penalty_cost_late</t>
+  </si>
+  <si>
+    <t>penalty_cost_not_performed</t>
+  </si>
+  <si>
+    <t>latest_period</t>
   </si>
 </sst>
 </file>
@@ -533,19 +551,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF71955-FB00-4A13-9841-9B985EEEFB62}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -555,8 +578,23 @@
       <c r="C1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>30</v>
       </c>
@@ -566,9 +604,25 @@
       <c r="C2">
         <v>30</v>
       </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+      <c r="E2">
+        <v>500</v>
+      </c>
+      <c r="F2">
+        <v>20000</v>
+      </c>
+      <c r="G2">
+        <v>1000000</v>
+      </c>
+      <c r="H2">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -577,7 +631,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -634,19 +688,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5129D5-4392-4795-B324-B7E69B03092B}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -674,8 +731,11 @@
       <c r="I1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -703,8 +763,11 @@
       <c r="I2">
         <v>10000</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -732,8 +795,11 @@
       <c r="I3">
         <v>80000</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -760,6 +826,9 @@
       </c>
       <c r="I4">
         <v>130000</v>
+      </c>
+      <c r="J4">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -772,10 +841,16 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -948,7 +1023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3E7950-5805-40E5-8CB7-09BB0C8D59D5}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
all Ivana's constraints implemented!
</commit_message>
<xml_diff>
--- a/data/Inputs.xlsx
+++ b/data/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3dd903d477a9e4d/02_ME/ME54015/OWF_Vessel-Fleet-Optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="207" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6287613-7D4E-4B18-B165-7B7CE9C12CF1}"/>
+  <xr:revisionPtr revIDLastSave="210" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F649A1C4-D109-43C1-AA6F-9E72C5A59C32}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="5" r:id="rId1"/>
@@ -553,7 +553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF71955-FB00-4A13-9841-9B985EEEFB62}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -690,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5129D5-4392-4795-B324-B7E69B03092B}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -758,7 +758,7 @@
         <v>5</v>
       </c>
       <c r="H2">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="I2">
         <v>10000</v>
@@ -790,7 +790,7 @@
         <v>4</v>
       </c>
       <c r="H3">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="I3">
         <v>80000</v>
@@ -822,7 +822,7 @@
         <v>2</v>
       </c>
       <c r="H4">
-        <v>24</v>
+        <v>240</v>
       </c>
       <c r="I4">
         <v>130000</v>

</xml_diff>

<commit_message>
Added the weather restrictions constraint
</commit_message>
<xml_diff>
--- a/data/Inputs.xlsx
+++ b/data/Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3dd903d477a9e4d/02_ME/ME54015/OWF_Vessel-Fleet-Optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="210" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F649A1C4-D109-43C1-AA6F-9E72C5A59C32}"/>
+  <xr:revisionPtr revIDLastSave="217" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5D70759-6E8C-4092-B64D-E63B18DDC02F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
   </bookViews>
@@ -691,7 +691,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -752,13 +752,13 @@
         <v>10</v>
       </c>
       <c r="F2">
-        <v>15</v>
+        <v>0.25</v>
       </c>
       <c r="G2">
         <v>5</v>
       </c>
       <c r="H2">
-        <v>120</v>
+        <v>12</v>
       </c>
       <c r="I2">
         <v>10000</v>
@@ -784,13 +784,14 @@
         <v>12</v>
       </c>
       <c r="F3">
-        <v>20</v>
+        <f>20/60</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G3">
         <v>4</v>
       </c>
       <c r="H3">
-        <v>120</v>
+        <v>12</v>
       </c>
       <c r="I3">
         <v>80000</v>
@@ -816,13 +817,14 @@
         <v>12</v>
       </c>
       <c r="F4">
-        <v>30</v>
+        <f>30/60</f>
+        <v>0.5</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="H4">
-        <v>240</v>
+        <v>24</v>
       </c>
       <c r="I4">
         <v>130000</v>

</xml_diff>

<commit_message>
Added spare parts set
</commit_message>
<xml_diff>
--- a/data/Inputs.xlsx
+++ b/data/Inputs.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3dd903d477a9e4d/02_ME/ME54015/OWF_Vessel-Fleet-Optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="217" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5D70759-6E8C-4092-B64D-E63B18DDC02F}"/>
+  <xr:revisionPtr revIDLastSave="229" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40820339-1358-4104-9704-C66A38C0CD8E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="5" r:id="rId1"/>
     <sheet name="bases" sheetId="1" r:id="rId2"/>
     <sheet name="vessels" sheetId="2" r:id="rId3"/>
     <sheet name="tasks" sheetId="3" r:id="rId4"/>
-    <sheet name="task_compatibility" sheetId="4" r:id="rId5"/>
-    <sheet name="capacity_base_vessels" sheetId="6" r:id="rId6"/>
+    <sheet name="spare_parts" sheetId="7" r:id="rId5"/>
+    <sheet name="task_compatibility" sheetId="4" r:id="rId6"/>
+    <sheet name="capacity_base_vessels" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>B1</t>
   </si>
@@ -174,6 +175,18 @@
   </si>
   <si>
     <t>latest_period</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
   </si>
 </sst>
 </file>
@@ -690,7 +703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5129D5-4392-4795-B324-B7E69B03092B}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -952,6 +965,46 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50264280-C602-45CD-AF71-2077C88A1536}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F60F74-5991-4DF7-ADB4-D8FEE6BDA60A}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -1021,7 +1074,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3E7950-5805-40E5-8CB7-09BB0C8D59D5}">
   <dimension ref="A1:D3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added the single-echelon parameters
</commit_message>
<xml_diff>
--- a/data/Inputs.xlsx
+++ b/data/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3dd903d477a9e4d/02_ME/ME54015/OWF_Vessel-Fleet-Optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="229" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40820339-1358-4104-9704-C66A38C0CD8E}"/>
+  <xr:revisionPtr revIDLastSave="294" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55F8D760-6162-40D4-8F4C-275699ACF7E5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="9" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="5" r:id="rId1"/>
@@ -20,6 +20,10 @@
     <sheet name="spare_parts" sheetId="7" r:id="rId5"/>
     <sheet name="task_compatibility" sheetId="4" r:id="rId6"/>
     <sheet name="capacity_base_vessels" sheetId="6" r:id="rId7"/>
+    <sheet name="holding_costs" sheetId="8" r:id="rId8"/>
+    <sheet name="spare_parts_required" sheetId="9" r:id="rId9"/>
+    <sheet name="max_capacity" sheetId="10" r:id="rId10"/>
+    <sheet name="reorder_level" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +46,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>B1</t>
   </si>
@@ -187,6 +191,12 @@
   </si>
   <si>
     <t>S4</t>
+  </si>
+  <si>
+    <t>order_cost</t>
+  </si>
+  <si>
+    <t>lead_time</t>
   </si>
 </sst>
 </file>
@@ -639,6 +649,144 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{053CB446-56D8-4850-8B54-9A701C7360FF}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="str" cm="1">
+        <f t="array" ref="B1:C1">TRANSPOSE(_xlfn._xlws.FILTER(bases!A2:A100, bases!A2:A100&lt;&gt;""))</f>
+        <v>B1</v>
+      </c>
+      <c r="C1" t="str">
+        <v>B2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2:A5">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
+        <v>S1</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <v>S2</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <v>S3</v>
+      </c>
+      <c r="B4">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <v>S4</v>
+      </c>
+      <c r="B5">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899CD8D2-6DC6-477C-BD52-3078DFB872A3}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="str" cm="1">
+        <f t="array" ref="B1:C1">TRANSPOSE(_xlfn._xlws.FILTER(bases!A2:A100, bases!A2:A100&lt;&gt;""))</f>
+        <v>B1</v>
+      </c>
+      <c r="C1" t="str">
+        <v>B2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2:A5">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
+        <v>S1</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <v>S2</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <v>S3</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <v>S4</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A06E241-D090-4C23-9A88-3F3C92E70F61}">
   <dimension ref="A1:D3"/>
@@ -966,37 +1114,67 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50264280-C602-45CD-AF71-2077C88A1536}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1079,7 +1257,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1128,4 +1306,157 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96EB2CC8-B9D8-4FE5-960B-9B0984034D8D}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="str" cm="1">
+        <f t="array" ref="B1:C1">TRANSPOSE(_xlfn._xlws.FILTER(bases!A2:A100, bases!A2:A100&lt;&gt;""))</f>
+        <v>B1</v>
+      </c>
+      <c r="C1" t="str">
+        <v>B2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2:A5">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
+        <v>S1</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <v>S2</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <v>S3</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <v>S4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397EDE46-A218-4D87-9847-C01D7AFA5102}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="str" cm="1">
+        <f t="array" ref="B1:D1">TRANSPOSE(_xlfn._xlws.FILTER(tasks!A2:A100, tasks!A2:A100&lt;&gt;""))</f>
+        <v>M1</v>
+      </c>
+      <c r="C1" t="str">
+        <v>M2</v>
+      </c>
+      <c r="D1" t="str">
+        <v>M3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2:A5">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
+        <v>S1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <v>S2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <v>S3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <v>S4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
all SE constraints added (infeasible)
</commit_message>
<xml_diff>
--- a/data/Inputs.xlsx
+++ b/data/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3dd903d477a9e4d/02_ME/ME54015/OWF_Vessel-Fleet-Optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="294" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55F8D760-6162-40D4-8F4C-275699ACF7E5}"/>
+  <xr:revisionPtr revIDLastSave="318" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0408067-4471-485E-855D-6C69C1560B13}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="9" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="9" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="5" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -654,7 +654,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,10 +674,10 @@
         <v>S1</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -685,10 +685,10 @@
         <v>S2</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -696,10 +696,10 @@
         <v>S3</v>
       </c>
       <c r="B4">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -707,10 +707,10 @@
         <v>S4</v>
       </c>
       <c r="B5">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -723,7 +723,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,10 +743,10 @@
         <v>S1</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -754,10 +754,10 @@
         <v>S2</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -765,10 +765,10 @@
         <v>S3</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -776,10 +776,10 @@
         <v>S4</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1116,7 +1116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50264280-C602-45CD-AF71-2077C88A1536}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
SE constraints: sort of work? not sure
</commit_message>
<xml_diff>
--- a/data/Inputs.xlsx
+++ b/data/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3dd903d477a9e4d/02_ME/ME54015/OWF_Vessel-Fleet-Optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="318" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0408067-4471-485E-855D-6C69C1560B13}"/>
+  <xr:revisionPtr revIDLastSave="326" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{042EA562-D850-49C5-BA8A-71054D69F932}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="9" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="8" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="5" r:id="rId1"/>
@@ -653,7 +653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{053CB446-56D8-4850-8B54-9A701C7360FF}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1381,8 +1381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397EDE46-A218-4D87-9847-C01D7AFA5102}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1405,7 +1405,7 @@
         <v>S1</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1419,13 +1419,13 @@
         <v>S2</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1436,7 +1436,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1447,13 +1447,13 @@
         <v>S4</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SE constraints, getting closer
</commit_message>
<xml_diff>
--- a/data/Inputs.xlsx
+++ b/data/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3dd903d477a9e4d/02_ME/ME54015/OWF_Vessel-Fleet-Optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="326" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{042EA562-D850-49C5-BA8A-71054D69F932}"/>
+  <xr:revisionPtr revIDLastSave="331" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8185416-1C93-4F3D-A75D-E033BCC4C3AE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="8" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="10" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="5" r:id="rId1"/>
@@ -722,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899CD8D2-6DC6-477C-BD52-3078DFB872A3}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,10 +743,10 @@
         <v>S1</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1381,7 +1381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397EDE46-A218-4D87-9847-C01D7AFA5102}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
SE constraints: forced re-order up to max capacity level --> optimization takes many hours now
</commit_message>
<xml_diff>
--- a/data/Inputs.xlsx
+++ b/data/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3dd903d477a9e4d/02_ME/ME54015/OWF_Vessel-Fleet-Optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="331" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8185416-1C93-4F3D-A75D-E033BCC4C3AE}"/>
+  <xr:revisionPtr revIDLastSave="341" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B50C7727-FF25-44B4-9F8F-D8744653D5D8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="10" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="9" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="5" r:id="rId1"/>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{053CB446-56D8-4850-8B54-9A701C7360FF}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,10 +674,10 @@
         <v>S1</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -685,10 +685,10 @@
         <v>S2</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C3">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -696,10 +696,10 @@
         <v>S3</v>
       </c>
       <c r="B4">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C4">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -707,10 +707,10 @@
         <v>S4</v>
       </c>
       <c r="B5">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C5">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -722,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899CD8D2-6DC6-477C-BD52-3078DFB872A3}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,10 +743,10 @@
         <v>S1</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Adding the latest versions of the code to grasp implementation (#4)
* Added spare parts set

* Added the single-echelon parameters

* Added the single-echelon variables

* Bring the file model/variables.py over from GRASP-implementation

* re-added the single-echelon variables

* all SE constraints added (infeasible)

* SE constraints: sort of work? not sure

* SE constraints, getting closer

* SE constraints: re-ordering works

* SE constraints: forced re-order up to max capacity level --> optimization takes many hours now

* SE constraints: All implemented
</commit_message>
<xml_diff>
--- a/data/Inputs.xlsx
+++ b/data/Inputs.xlsx
@@ -8,17 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3dd903d477a9e4d/02_ME/ME54015/OWF_Vessel-Fleet-Optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="217" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5D70759-6E8C-4092-B64D-E63B18DDC02F}"/>
+  <xr:revisionPtr revIDLastSave="341" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B50C7727-FF25-44B4-9F8F-D8744653D5D8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="9" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="5" r:id="rId1"/>
     <sheet name="bases" sheetId="1" r:id="rId2"/>
     <sheet name="vessels" sheetId="2" r:id="rId3"/>
     <sheet name="tasks" sheetId="3" r:id="rId4"/>
-    <sheet name="task_compatibility" sheetId="4" r:id="rId5"/>
-    <sheet name="capacity_base_vessels" sheetId="6" r:id="rId6"/>
+    <sheet name="spare_parts" sheetId="7" r:id="rId5"/>
+    <sheet name="task_compatibility" sheetId="4" r:id="rId6"/>
+    <sheet name="capacity_base_vessels" sheetId="6" r:id="rId7"/>
+    <sheet name="holding_costs" sheetId="8" r:id="rId8"/>
+    <sheet name="spare_parts_required" sheetId="9" r:id="rId9"/>
+    <sheet name="max_capacity" sheetId="10" r:id="rId10"/>
+    <sheet name="reorder_level" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>B1</t>
   </si>
@@ -174,6 +179,24 @@
   </si>
   <si>
     <t>latest_period</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>order_cost</t>
+  </si>
+  <si>
+    <t>lead_time</t>
   </si>
 </sst>
 </file>
@@ -626,6 +649,144 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{053CB446-56D8-4850-8B54-9A701C7360FF}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="str" cm="1">
+        <f t="array" ref="B1:C1">TRANSPOSE(_xlfn._xlws.FILTER(bases!A2:A100, bases!A2:A100&lt;&gt;""))</f>
+        <v>B1</v>
+      </c>
+      <c r="C1" t="str">
+        <v>B2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2:A5">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
+        <v>S1</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <v>S2</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <v>S3</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <v>S4</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899CD8D2-6DC6-477C-BD52-3078DFB872A3}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="str" cm="1">
+        <f t="array" ref="B1:C1">TRANSPOSE(_xlfn._xlws.FILTER(bases!A2:A100, bases!A2:A100&lt;&gt;""))</f>
+        <v>B1</v>
+      </c>
+      <c r="C1" t="str">
+        <v>B2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2:A5">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
+        <v>S1</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <v>S2</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <v>S3</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <v>S4</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A06E241-D090-4C23-9A88-3F3C92E70F61}">
   <dimension ref="A1:D3"/>
@@ -690,7 +851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5129D5-4392-4795-B324-B7E69B03092B}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -952,6 +1113,76 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50264280-C602-45CD-AF71-2077C88A1536}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F60F74-5991-4DF7-ADB4-D8FEE6BDA60A}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -1021,12 +1252,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3E7950-5805-40E5-8CB7-09BB0C8D59D5}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1075,4 +1306,157 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96EB2CC8-B9D8-4FE5-960B-9B0984034D8D}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="str" cm="1">
+        <f t="array" ref="B1:C1">TRANSPOSE(_xlfn._xlws.FILTER(bases!A2:A100, bases!A2:A100&lt;&gt;""))</f>
+        <v>B1</v>
+      </c>
+      <c r="C1" t="str">
+        <v>B2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2:A5">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
+        <v>S1</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <v>S2</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <v>S3</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <v>S4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397EDE46-A218-4D87-9847-C01D7AFA5102}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="str" cm="1">
+        <f t="array" ref="B1:D1">TRANSPOSE(_xlfn._xlws.FILTER(tasks!A2:A100, tasks!A2:A100&lt;&gt;""))</f>
+        <v>M1</v>
+      </c>
+      <c r="C1" t="str">
+        <v>M2</v>
+      </c>
+      <c r="D1" t="str">
+        <v>M3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2:A5">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
+        <v>S1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <v>S2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <v>S3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <v>S4</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Greedy construction algorithm done
</commit_message>
<xml_diff>
--- a/data/Inputs.xlsx
+++ b/data/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3dd903d477a9e4d/02_ME/ME54015/OWF_Vessel-Fleet-Optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="341" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B50C7727-FF25-44B4-9F8F-D8744653D5D8}"/>
+  <xr:revisionPtr revIDLastSave="342" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D9C53AE-5D15-47F8-9EEB-51730F1FED0F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="9" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="5" r:id="rId1"/>
@@ -653,7 +653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{053CB446-56D8-4850-8B54-9A701C7360FF}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -851,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5129D5-4392-4795-B324-B7E69B03092B}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -913,6 +913,7 @@
         <v>10</v>
       </c>
       <c r="F2">
+        <f>15/60</f>
         <v>0.25</v>
       </c>
       <c r="G2">

</xml_diff>

<commit_message>
deGooijer25 Initial Model is verified
</commit_message>
<xml_diff>
--- a/data/Inputs.xlsx
+++ b/data/Inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3dd903d477a9e4d/02_ME/ME54015/OWF_Vessel-Fleet-Optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="342" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D9C53AE-5D15-47F8-9EEB-51730F1FED0F}"/>
+  <xr:revisionPtr revIDLastSave="348" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6837B80E-2CAA-43F1-9D7F-9CFDAF6D5302}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
   </bookViews>
@@ -852,7 +852,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -907,7 +907,7 @@
         <v>20</v>
       </c>
       <c r="D2">
-        <v>5000</v>
+        <v>166.67</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -926,7 +926,7 @@
         <v>10000</v>
       </c>
       <c r="J2">
-        <v>100</v>
+        <v>166.67</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -940,7 +940,7 @@
         <v>30</v>
       </c>
       <c r="D3">
-        <v>10000</v>
+        <v>333.33</v>
       </c>
       <c r="E3">
         <v>12</v>
@@ -959,7 +959,7 @@
         <v>80000</v>
       </c>
       <c r="J3">
-        <v>100</v>
+        <v>166.67</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -973,7 +973,7 @@
         <v>25</v>
       </c>
       <c r="D4">
-        <v>16250</v>
+        <v>541.66999999999996</v>
       </c>
       <c r="E4">
         <v>12</v>
@@ -992,7 +992,7 @@
         <v>130000</v>
       </c>
       <c r="J4">
-        <v>100</v>
+        <v>83.33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
plotter now better, good results for verification possible
</commit_message>
<xml_diff>
--- a/data/Inputs.xlsx
+++ b/data/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3dd903d477a9e4d/02_ME/ME54015/OWF_Vessel-Fleet-Optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="348" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6837B80E-2CAA-43F1-9D7F-9CFDAF6D5302}"/>
+  <xr:revisionPtr revIDLastSave="359" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5287B7C5-350C-4629-A789-7FAD9FD6FABB}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="10" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="5" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>B1</t>
   </si>
@@ -185,12 +185,6 @@
   </si>
   <si>
     <t>S2</t>
-  </si>
-  <si>
-    <t>S3</t>
-  </si>
-  <si>
-    <t>S4</t>
   </si>
   <si>
     <t>order_cost</t>
@@ -654,7 +648,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,14 +664,14 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A5">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
+        <f t="array" ref="A2:A3">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
         <v>S1</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -685,16 +679,13 @@
         <v>S2</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
-        <v>S3</v>
-      </c>
       <c r="B4">
         <v>20</v>
       </c>
@@ -703,9 +694,6 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <v>S4</v>
-      </c>
       <c r="B5">
         <v>20</v>
       </c>
@@ -722,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899CD8D2-6DC6-477C-BD52-3078DFB872A3}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,7 +727,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A5">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
+        <f t="array" ref="A2:A3">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
         <v>S1</v>
       </c>
       <c r="B2">
@@ -761,9 +749,6 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
-        <v>S3</v>
-      </c>
       <c r="B4">
         <v>10</v>
       </c>
@@ -772,9 +757,6 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <v>S4</v>
-      </c>
       <c r="B5">
         <v>10</v>
       </c>
@@ -851,7 +833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5129D5-4392-4795-B324-B7E69B03092B}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1115,10 +1097,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50264280-C602-45CD-AF71-2077C88A1536}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1128,10 +1110,10 @@
         <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1154,28 +1136,6 @@
       </c>
       <c r="C3">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4">
-        <v>30</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5">
-        <v>40</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1314,7 +1274,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1330,14 +1290,14 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A5">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
+        <f t="array" ref="A2:A3">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
         <v>S1</v>
       </c>
       <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
         <v>5</v>
-      </c>
-      <c r="C2">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1345,16 +1305,13 @@
         <v>S2</v>
       </c>
       <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
-        <v>S3</v>
-      </c>
       <c r="B4">
         <v>4</v>
       </c>
@@ -1363,9 +1320,6 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <v>S4</v>
-      </c>
       <c r="B5">
         <v>2</v>
       </c>
@@ -1383,7 +1337,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1402,14 +1356,14 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A5">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
+        <f t="array" ref="A2:A3">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
         <v>S1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1423,16 +1377,13 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
-        <v>S3</v>
-      </c>
       <c r="B4">
         <v>0</v>
       </c>
@@ -1444,9 +1395,6 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <v>S4</v>
-      </c>
       <c r="B5">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added all sets, params, vars and data except for the technician flows
</commit_message>
<xml_diff>
--- a/data/Inputs.xlsx
+++ b/data/Inputs.xlsx
@@ -5,25 +5,27 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3dd903d477a9e4d/02_ME/ME54015/OWF_Vessel-Fleet-Optimization/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liams\OneDrive\Documents\Mischa Code\OWF_Vessel-Fleet-Optimization\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="348" documentId="8_{D235DB62-0293-48F4-BA36-F64F0C452A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6837B80E-2CAA-43F1-9D7F-9CFDAF6D5302}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3151CD22-8B3E-4FC5-8CCE-42E55EA3313D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="5" r:id="rId1"/>
     <sheet name="bases" sheetId="1" r:id="rId2"/>
     <sheet name="vessels" sheetId="2" r:id="rId3"/>
-    <sheet name="tasks" sheetId="3" r:id="rId4"/>
-    <sheet name="spare_parts" sheetId="7" r:id="rId5"/>
-    <sheet name="task_compatibility" sheetId="4" r:id="rId6"/>
-    <sheet name="capacity_base_vessels" sheetId="6" r:id="rId7"/>
-    <sheet name="holding_costs" sheetId="8" r:id="rId8"/>
-    <sheet name="spare_parts_required" sheetId="9" r:id="rId9"/>
-    <sheet name="max_capacity" sheetId="10" r:id="rId10"/>
-    <sheet name="reorder_level" sheetId="11" r:id="rId11"/>
+    <sheet name="mother_vessels" sheetId="13" r:id="rId4"/>
+    <sheet name="locations" sheetId="12" r:id="rId5"/>
+    <sheet name="tasks" sheetId="3" r:id="rId6"/>
+    <sheet name="spare_parts" sheetId="7" r:id="rId7"/>
+    <sheet name="task_compatibility" sheetId="4" r:id="rId8"/>
+    <sheet name="capacity_base_vessels" sheetId="6" r:id="rId9"/>
+    <sheet name="holding_costs" sheetId="8" r:id="rId10"/>
+    <sheet name="spare_parts_required" sheetId="9" r:id="rId11"/>
+    <sheet name="max_capacity" sheetId="10" r:id="rId12"/>
+    <sheet name="reorder_level" sheetId="11" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -68,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>B1</t>
   </si>
@@ -187,16 +189,25 @@
     <t>S2</t>
   </si>
   <si>
-    <t>S3</t>
-  </si>
-  <si>
-    <t>S4</t>
-  </si>
-  <si>
     <t>order_cost</t>
   </si>
   <si>
     <t>lead_time</t>
+  </si>
+  <si>
+    <t>MV</t>
+  </si>
+  <si>
+    <t>V4</t>
+  </si>
+  <si>
+    <t>max_capacity_for_docking</t>
+  </si>
+  <si>
+    <t>additional_time</t>
+  </si>
+  <si>
+    <t>tech_standby_cost</t>
   </si>
 </sst>
 </file>
@@ -574,24 +585,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF71955-FB00-4A13-9841-9B985EEEFB62}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.5234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7890625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.20703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.20703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.68359375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.3125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -616,8 +628,11 @@
       <c r="H1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>30</v>
       </c>
@@ -641,6 +656,9 @@
       </c>
       <c r="H2">
         <v>80</v>
+      </c>
+      <c r="I2">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -650,67 +668,661 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96EB2CC8-B9D8-4FE5-960B-9B0984034D8D}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="str" cm="1">
+        <f t="array" ref="B1:D1">TRANSPOSE(_xlfn._xlws.FILTER(locations!A2:A100, locations!A2:A100&lt;&gt;""))</f>
+        <v>B1</v>
+      </c>
+      <c r="C1" t="str">
+        <v>B2</v>
+      </c>
+      <c r="D1" t="str">
+        <v>V4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2:A3">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
+        <v>S1</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="str">
+        <v>S2</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397EDE46-A218-4D87-9847-C01D7AFA5102}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="str" cm="1">
+        <f t="array" ref="B1:D1">TRANSPOSE(_xlfn._xlws.FILTER(tasks!A2:A100, tasks!A2:A100&lt;&gt;""))</f>
+        <v>M1</v>
+      </c>
+      <c r="C1" t="str">
+        <v>M2</v>
+      </c>
+      <c r="D1" t="str">
+        <v>M3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2:A3">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
+        <v>S1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="str">
+        <v>S2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{053CB446-56D8-4850-8B54-9A701C7360FF}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="str" cm="1">
+        <f t="array" ref="B1:D1">TRANSPOSE(_xlfn._xlws.FILTER(locations!A2:A100, locations!A2:A100&lt;&gt;""))</f>
+        <v>B1</v>
+      </c>
+      <c r="C1" t="str">
+        <v>B2</v>
+      </c>
+      <c r="D1" t="str">
+        <v>V4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2:A3">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
+        <v>S1</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="str">
+        <v>S2</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899CD8D2-6DC6-477C-BD52-3078DFB872A3}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="str" cm="1">
+        <f t="array" ref="B1:D1">TRANSPOSE(_xlfn._xlws.FILTER(locations!A2:A100, locations!A2:A100&lt;&gt;""))</f>
+        <v>B1</v>
+      </c>
+      <c r="C1" t="str">
+        <v>B2</v>
+      </c>
+      <c r="D1" t="str">
+        <v>V4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2:A3">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
+        <v>S1</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="str">
+        <v>S2</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A06E241-D090-4C23-9A88-3F3C92E70F61}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="8.89453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>60</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>550000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>80</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>450000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5129D5-4392-4795-B324-B7E69B03092B}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="5" max="5" width="14.7890625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.20703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7890625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5234375" customWidth="1"/>
+    <col min="12" max="12" width="12.7890625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>166.67</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <f>15/60</f>
+        <v>0.25</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>12</v>
+      </c>
+      <c r="J2">
+        <v>10000</v>
+      </c>
+      <c r="K2">
+        <v>166.67</v>
+      </c>
+      <c r="L2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>2.5</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="E3">
+        <v>333.33</v>
+      </c>
+      <c r="F3">
+        <v>12</v>
+      </c>
+      <c r="G3">
+        <f>20/60</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>12</v>
+      </c>
+      <c r="J3">
+        <v>80000</v>
+      </c>
+      <c r="K3">
+        <v>166.67</v>
+      </c>
+      <c r="L3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <v>541.66999999999996</v>
+      </c>
+      <c r="F4">
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <f>30/60</f>
+        <v>0.5</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>24</v>
+      </c>
+      <c r="J4">
+        <v>130000</v>
+      </c>
+      <c r="K4">
+        <v>83.33</v>
+      </c>
+      <c r="L4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <v>800</v>
+      </c>
+      <c r="F5">
+        <v>40</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>168</v>
+      </c>
+      <c r="J5">
+        <v>300000</v>
+      </c>
+      <c r="K5">
+        <v>50</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E60961F4-8CE3-4B3A-93AF-60EFCE35F0D1}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2">_xlfn._xlws.FILTER(vessels!A2:A100, vessels!B2:B100 = 1)</f>
+        <v>V4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EABC1D42-2EA6-4A74-ACE3-149C8A508F63}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="3" max="3" width="21.3125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:C1">TRANSPOSE(_xlfn._xlws.FILTER(bases!A2:A100, bases!A2:A100&lt;&gt;""))</f>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2:A4">_xlfn.LET(
+    _xlpm.baseList, _xlfn._xlws.FILTER(bases!A2:A100, bases!A2:A100 &lt;&gt; ""),
+    _xlpm.vesselList, _xlfn._xlws.FILTER(vessels!A2:A100, vessels!B2:B100 = 1),
+    _xlfn.VSTACK(_xlpm.baseList, _xlpm.vesselList)
+)</f>
         <v>B1</v>
       </c>
-      <c r="C1" t="str">
+      <c r="B2">
+        <v>60</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="str">
         <v>B2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A5">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
-        <v>S1</v>
-      </c>
-      <c r="B2">
-        <v>20</v>
-      </c>
-      <c r="C2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <v>S2</v>
-      </c>
       <c r="B3">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="C3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="str">
-        <v>S3</v>
+        <v>V4</v>
       </c>
       <c r="B4">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <v>S4</v>
-      </c>
-      <c r="B5">
-        <v>20</v>
-      </c>
-      <c r="C5">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -718,289 +1330,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899CD8D2-6DC6-477C-BD52-3078DFB872A3}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:C1">TRANSPOSE(_xlfn._xlws.FILTER(bases!A2:A100, bases!A2:A100&lt;&gt;""))</f>
-        <v>B1</v>
-      </c>
-      <c r="C1" t="str">
-        <v>B2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A5">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
-        <v>S1</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <v>S2</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
-        <v>S3</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <v>S4</v>
-      </c>
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A06E241-D090-4C23-9A88-3F3C92E70F61}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>60</v>
-      </c>
-      <c r="C2">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>550000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>80</v>
-      </c>
-      <c r="C3">
-        <v>16</v>
-      </c>
-      <c r="D3">
-        <v>450000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5129D5-4392-4795-B324-B7E69B03092B}">
-  <dimension ref="A1:J4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>166.67</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <f>15/60</f>
-        <v>0.25</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <v>12</v>
-      </c>
-      <c r="I2">
-        <v>10000</v>
-      </c>
-      <c r="J2">
-        <v>166.67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>2.5</v>
-      </c>
-      <c r="C3">
-        <v>30</v>
-      </c>
-      <c r="D3">
-        <v>333.33</v>
-      </c>
-      <c r="E3">
-        <v>12</v>
-      </c>
-      <c r="F3">
-        <f>20/60</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>12</v>
-      </c>
-      <c r="I3">
-        <v>80000</v>
-      </c>
-      <c r="J3">
-        <v>166.67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="C4">
-        <v>25</v>
-      </c>
-      <c r="D4">
-        <v>541.66999999999996</v>
-      </c>
-      <c r="E4">
-        <v>12</v>
-      </c>
-      <c r="F4">
-        <f>30/60</f>
-        <v>0.5</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>24</v>
-      </c>
-      <c r="I4">
-        <v>130000</v>
-      </c>
-      <c r="J4">
-        <v>83.33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF4AD3B-D68B-43E0-80DF-E258B870C86F}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -1008,15 +1338,15 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1015625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1039,7 +1369,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1062,7 +1392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1085,7 +1415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1113,28 +1443,28 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50264280-C602-45CD-AF71-2077C88A1536}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1145,7 +1475,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1156,10 +1486,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B4">
         <v>30</v>
       </c>
@@ -1167,10 +1494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>40</v>
-      </c>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B5">
         <v>40</v>
       </c>
@@ -1183,19 +1507,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F60F74-5991-4DF7-ADB4-D8FEE6BDA60A}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:D1">TRANSPOSE(_xlfn._xlws.FILTER(vessels!A2:A100, vessels!A2:A100&lt;&gt;""))</f>
+        <f t="array" ref="B1:E1">TRANSPOSE(_xlfn._xlws.FILTER(vessels!A2:A100, vessels!A2:A100&lt;&gt;""))</f>
         <v>V1</v>
       </c>
       <c r="C1" t="str">
@@ -1204,8 +1528,11 @@
       <c r="D1" t="str">
         <v>V3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="str">
+        <v>V4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="str" cm="1">
         <f t="array" ref="A2:A4">_xlfn._xlws.FILTER(tasks!A2:A100, tasks!A2:A100&lt;&gt;"")</f>
         <v>M1</v>
@@ -1219,8 +1546,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="str">
         <v>M2</v>
       </c>
@@ -1233,8 +1563,11 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="str">
         <v>M3</v>
       </c>
@@ -1246,6 +1579,9 @@
       </c>
       <c r="D4">
         <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1253,19 +1589,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3E7950-5805-40E5-8CB7-09BB0C8D59D5}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:D1">TRANSPOSE(_xlfn._xlws.FILTER(vessels!A2:A100, vessels!A2:A100&lt;&gt;""))</f>
+        <f t="array" ref="B1:E1">TRANSPOSE(_xlfn._xlws.FILTER(vessels!A2:A100, vessels!A2:A100&lt;&gt;""))</f>
         <v>V1</v>
       </c>
       <c r="C1" t="str">
@@ -1274,8 +1610,11 @@
       <c r="D1" t="str">
         <v>V3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="str">
+        <v>V4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="str" cm="1">
         <f t="array" ref="A2:A3">_xlfn._xlws.FILTER(bases!A2:A100, bases!A2:A100&lt;&gt;"")</f>
         <v>B1</v>
@@ -1289,8 +1628,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="str">
         <v>B2</v>
       </c>
@@ -1303,158 +1645,8 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96EB2CC8-B9D8-4FE5-960B-9B0984034D8D}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:C1">TRANSPOSE(_xlfn._xlws.FILTER(bases!A2:A100, bases!A2:A100&lt;&gt;""))</f>
-        <v>B1</v>
-      </c>
-      <c r="C1" t="str">
-        <v>B2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A5">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
-        <v>S1</v>
-      </c>
-      <c r="B2">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <v>S2</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
-        <v>S3</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <v>S4</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397EDE46-A218-4D87-9847-C01D7AFA5102}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:D1">TRANSPOSE(_xlfn._xlws.FILTER(tasks!A2:A100, tasks!A2:A100&lt;&gt;""))</f>
-        <v>M1</v>
-      </c>
-      <c r="C1" t="str">
-        <v>M2</v>
-      </c>
-      <c r="D1" t="str">
-        <v>M3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A5">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
-        <v>S1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <v>S2</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
-        <v>S3</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <v>S4</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
+      <c r="E3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First constraints added SE
</commit_message>
<xml_diff>
--- a/data/Inputs.xlsx
+++ b/data/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liams\OneDrive\Documents\Mischa Code\OWF_Vessel-Fleet-Optimization\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3151CD22-8B3E-4FC5-8CCE-42E55EA3313D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E655DA3-6644-44D5-B8A3-390376DF86AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" firstSheet="8" activeTab="12" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="5" r:id="rId1"/>
@@ -587,7 +587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF71955-FB00-4A13-9841-9B985EEEFB62}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -669,10 +669,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96EB2CC8-B9D8-4FE5-960B-9B0984034D8D}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B4" sqref="B4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -718,22 +718,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -741,10 +725,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397EDE46-A218-4D87-9847-C01D7AFA5102}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B4" sqref="B4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -790,28 +774,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -819,10 +781,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{053CB446-56D8-4850-8B54-9A701C7360FF}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B4" sqref="B4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -868,22 +830,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4">
-        <v>20</v>
-      </c>
-      <c r="C4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5">
-        <v>20</v>
-      </c>
-      <c r="C5">
-        <v>20</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -891,10 +837,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899CD8D2-6DC6-477C-BD52-3078DFB872A3}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -938,22 +884,6 @@
       </c>
       <c r="D3">
         <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1445,10 +1375,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50264280-C602-45CD-AF71-2077C88A1536}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B4" sqref="B4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1484,22 +1414,6 @@
       </c>
       <c r="C3">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4">
-        <v>30</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5">
-        <v>40</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added mv operation cost
</commit_message>
<xml_diff>
--- a/data/Inputs.xlsx
+++ b/data/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3dd903d477a9e4d/02_ME/ME54015/OWF_Vessel-Fleet-Optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{4E655DA3-6644-44D5-B8A3-390376DF86AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1EAECED-A938-4583-B660-6DBDA9B4E6EC}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{4E655DA3-6644-44D5-B8A3-390376DF86AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0110E293-A9DF-450A-9249-8823A091FF35}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="10" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="5" r:id="rId1"/>
@@ -727,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397EDE46-A218-4D87-9847-C01D7AFA5102}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -751,10 +751,10 @@
         <v>S1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -768,7 +768,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -956,7 +956,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1043,7 +1043,7 @@
         <v>166.67</v>
       </c>
       <c r="L2">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1153,7 +1153,7 @@
         <v>168</v>
       </c>
       <c r="J5">
-        <v>300000</v>
+        <v>10000</v>
       </c>
       <c r="K5">
         <v>50</v>
@@ -1197,7 +1197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EABC1D42-2EA6-4A74-ACE3-149C8A508F63}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Lead time to 1
</commit_message>
<xml_diff>
--- a/data/Inputs.xlsx
+++ b/data/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3dd903d477a9e4d/02_ME/ME54015/OWF_Vessel-Fleet-Optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="259" documentId="13_ncr:1_{4E655DA3-6644-44D5-B8A3-390376DF86AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AA87C73-17E4-4A87-8EBA-1B0FCEEA7020}"/>
+  <xr:revisionPtr revIDLastSave="261" documentId="13_ncr:1_{4E655DA3-6644-44D5-B8A3-390376DF86AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD1C8517-43F0-449F-AB18-7B4EA23ED26E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="853" activeTab="6" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="853" activeTab="6" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="5" r:id="rId1"/>
@@ -576,19 +576,19 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -617,7 +617,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>30</v>
       </c>
@@ -660,9 +660,9 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="str" cm="1">
         <f t="array" ref="B1:D1">TRANSPOSE(_xlfn._xlws.FILTER(locations!A2:A100, locations!A2:A100&lt;&gt;""))</f>
         <v>B1</v>
@@ -674,7 +674,7 @@
         <v>V4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="str" cm="1">
         <f t="array" ref="A2">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
         <v>S1</v>
@@ -702,15 +702,15 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="str" cm="1">
         <f t="array" ref="B1">TRANSPOSE(_xlfn._xlws.FILTER(tasks!A2:A100, tasks!A2:A100&lt;&gt;""))</f>
         <v>M1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="str" cm="1">
         <f t="array" ref="A2">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
         <v>S1</v>
@@ -732,9 +732,9 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="str" cm="1">
         <f t="array" ref="B1:D1">TRANSPOSE(_xlfn._xlws.FILTER(locations!A2:A100, locations!A2:A100&lt;&gt;""))</f>
         <v>B1</v>
@@ -746,7 +746,7 @@
         <v>V4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="str" cm="1">
         <f t="array" ref="A2">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
         <v>S1</v>
@@ -774,9 +774,9 @@
       <selection activeCell="B3" sqref="B3:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="str" cm="1">
         <f t="array" ref="B1:D1">TRANSPOSE(_xlfn._xlws.FILTER(locations!A2:A100, locations!A2:A100&lt;&gt;""))</f>
         <v>B1</v>
@@ -788,7 +788,7 @@
         <v>V4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="str" cm="1">
         <f t="array" ref="A2">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
         <v>S1</v>
@@ -816,13 +816,13 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -836,7 +836,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -850,7 +850,7 @@
         <v>550000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -877,17 +877,17 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5546875" customWidth="1"/>
-    <col min="12" max="12" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -925,7 +925,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -964,7 +964,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
     </row>
   </sheetData>
@@ -1018,17 +1018,17 @@
       <selection activeCell="B1" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str" cm="1">
         <f t="array" ref="A2">_xlfn._xlws.FILTER(vessels!A2:A100, vessels!B2:B100 = 1)</f>
         <v>V4</v>
@@ -1047,14 +1047,14 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="str" cm="1">
         <f t="array" ref="A2:A4">_xlfn.LET(
     _xlpm.baseList, _xlfn._xlws.FILTER(bases!A2:A100, bases!A2:A100 &lt;&gt; ""),
@@ -1093,7 +1093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <v>B2</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <v>V4</v>
       </c>
@@ -1140,15 +1140,15 @@
       <selection activeCell="A3" sqref="A3:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1204,12 +1204,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1241,12 +1241,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="str" cm="1">
         <f t="array" ref="B1:C1">TRANSPOSE(_xlfn._xlws.FILTER(vessels!A2:A100, vessels!A2:A100&lt;&gt;""))</f>
         <v>V1</v>
@@ -1255,7 +1255,7 @@
         <v>V4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="str" cm="1">
         <f t="array" ref="A2">_xlfn._xlws.FILTER(tasks!A2:A100, tasks!A2:A100&lt;&gt;"")</f>
         <v>M1</v>
@@ -1280,9 +1280,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="str" cm="1">
         <f t="array" ref="B1:C1">TRANSPOSE(_xlfn._xlws.FILTER(vessels!A2:A100, vessels!A2:A100&lt;&gt;""))</f>
         <v>V1</v>
@@ -1291,7 +1291,7 @@
         <v>V4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="str" cm="1">
         <f t="array" ref="A2:A3">_xlfn._xlws.FILTER(bases!A2:A100, bases!A2:A100&lt;&gt;"")</f>
         <v>B1</v>
@@ -1303,7 +1303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <v>B2</v>
       </c>

</xml_diff>

<commit_message>
Initial solution for the verification case
</commit_message>
<xml_diff>
--- a/data/Inputs.xlsx
+++ b/data/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3dd903d477a9e4d/02_ME/ME54015/OWF_Vessel-Fleet-Optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="274" documentId="13_ncr:1_{4E655DA3-6644-44D5-B8A3-390376DF86AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB8D8D10-8A87-481A-9FE0-5A7612427556}"/>
+  <xr:revisionPtr revIDLastSave="276" documentId="13_ncr:1_{4E655DA3-6644-44D5-B8A3-390376DF86AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B94AC570-58BD-4071-B322-0F83A50A0FE5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="853" activeTab="4" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="853" activeTab="9" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="5" r:id="rId1"/>
@@ -656,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96EB2CC8-B9D8-4FE5-960B-9B0984034D8D}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1043,7 +1043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EABC1D42-2EA6-4A74-ACE3-149C8A508F63}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>